<commit_message>
finished govexec, moving to fednewsnet
</commit_message>
<xml_diff>
--- a/fed-events/Fed_Events-03.03.23.xlsx
+++ b/fed-events/Fed_Events-03.03.23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorcas/Development/python_scraper_parser_projects/fed-events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF1239E-4383-8145-B6C8-D4704A3916E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6685A637-136D-1D4B-90A7-C936BDE1BAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="26880" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FedScoop" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="187">
   <si>
     <t>Event Name</t>
   </si>
@@ -981,16 +981,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1153,13 +1150,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.5" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="116.83203125" bestFit="1" customWidth="1"/>
@@ -1372,7 +1369,7 @@
         <v>129</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1386,7 +1383,7 @@
         <v>129</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1400,7 +1397,7 @@
         <v>129</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1414,7 +1411,7 @@
         <v>130</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1428,7 +1425,7 @@
         <v>131</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1442,7 +1439,7 @@
         <v>132</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1456,7 +1453,7 @@
         <v>132</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1470,7 +1467,7 @@
         <v>133</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1484,7 +1481,7 @@
         <v>134</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1498,7 +1495,7 @@
         <v>135</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1512,7 +1509,7 @@
         <v>136</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1526,7 +1523,7 @@
         <v>137</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1540,7 +1537,7 @@
         <v>138</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1554,7 +1551,7 @@
         <v>138</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1568,7 +1565,7 @@
         <v>139</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1582,7 +1579,7 @@
         <v>139</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1596,7 +1593,7 @@
         <v>140</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1610,7 +1607,7 @@
         <v>141</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1624,7 +1621,7 @@
         <v>142</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1638,7 +1635,7 @@
         <v>125</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1652,7 +1649,7 @@
         <v>122</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1666,7 +1663,7 @@
         <v>143</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1680,7 +1677,7 @@
         <v>144</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1694,7 +1691,7 @@
         <v>145</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1708,7 +1705,7 @@
         <v>146</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1721,6 +1718,9 @@
       <c r="C40" t="s">
         <v>147</v>
       </c>
+      <c r="D40" s="2" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -1732,6 +1732,9 @@
       <c r="C41" t="s">
         <v>148</v>
       </c>
+      <c r="D41" s="2" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -1742,6 +1745,9 @@
       </c>
       <c r="C42" t="s">
         <v>149</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1784,6 +1790,9 @@
     <hyperlink ref="D37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
     <hyperlink ref="D38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
     <hyperlink ref="D39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="D40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="D41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="D42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updates to fed parsers
</commit_message>
<xml_diff>
--- a/fed-events/Fed_Events-03.03.23.xlsx
+++ b/fed-events/Fed_Events-03.03.23.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorcas/Development/python_scraper_parser_projects/fed-events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6685A637-136D-1D4B-90A7-C936BDE1BAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2700A0D3-7041-2241-9CBE-130850D7C330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="26880" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FedScoop" sheetId="1" r:id="rId1"/>
     <sheet name="Gov Exec" sheetId="2" r:id="rId2"/>
+    <sheet name="Nextgov" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="187">
   <si>
     <t>Event Name</t>
   </si>
@@ -981,13 +982,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1150,13 +1154,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="1" max="1" width="59.5" customWidth="1"/>
     <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="116.83203125" bestFit="1" customWidth="1"/>
@@ -1796,4 +1798,86 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>